<commit_message>
build logistic regression model
</commit_message>
<xml_diff>
--- a/Paper List.xlsx
+++ b/Paper List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Ava\1.PBCPDA\6 Semester 6\Machine Learning Techniques_EI Sayed Mahmoud\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE3969E-06DE-4640-9657-9F302299A154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E921FA-3162-4570-B5A5-D62569B2EDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t>Title</t>
   </si>
@@ -427,12 +427,71 @@
       <t xml:space="preserve"> are applied on it. The wine will be classified into three main categories and the accuracy of the algorithms are compared.</t>
     </r>
   </si>
+  <si>
+    <t>An SVM Based Wine Superiority Estimation Using Advanced ML Techniques</t>
+  </si>
+  <si>
+    <t>https://searchlibrary.sheridancollege.ca/discovery/fulldisplay?docid=cdi_proquest_journals_2637448844&amp;context=PC&amp;vid=01OCLS_SHER:SHER&amp;lang=en&amp;search_scope=MyInst_and_CI&amp;adaptor=Primo%20Central&amp;tab=Everything&amp;query=any,contains,wine%20using%20ML&amp;offset=0</t>
+  </si>
+  <si>
+    <t>Sirivanth, P., Krishna Rao, N. V., Manduva, J., Sekhar, G. C., Tajeswi, M., Veeresh, C., &amp; Kaushik, J. V. (2021). A SVM Based Wine Superiority Estimatation Using Advanced ML Techniques. 2021 3rd International Conference on Advances in Computing, Communication Control and Networking (ICAC3N), 207–211. https://doi.org/10.1109/ICAC3N53548.2021.9725492</t>
+  </si>
+  <si>
+    <t>Evaluation of Volatile Metabolites Emitted In-Vivo from Cold-Hardy Grapes during Ripening Using SPME and GC-MS: A Proof-of-Concept</t>
+  </si>
+  <si>
+    <t>https://www.proquest.com/docview/2548939910?pq-origsite=primo&amp;sourcetype=Scholarly%20Journals</t>
+  </si>
+  <si>
+    <t>Rice, S., Maurer, D. L., Fennell, A., Dharmadhikari, M., &amp; Koziel, J. A. (2019). Evaluation of volatile metabolites emitted in-vivo from cold-hardy grapes during ripening using SPME and GC-MS: A proof-of-concept. Molecules, 24(3), 536. doi:https://doi.org/10.3390/molecules24030536</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wine is one of the popular drinks as its consumption is quite popular among generations and the quality is dependent of time generally older the wine better the taste. One of the growing research areas in the field of engineering is machine learning. The current research emphasizes on the study of wine quality and class attributes using machine learning algorithms on Wine quality dataset. The quality of Wine contains different characteristics along with alcohol content found in it. The fluctuating nature of characteristics also defines variation, improvements received in quality of wine with reference to time horizon. Machine learning techniques are used to assess the quality under the dimension of different classification and regression methods to seek out higher accuracy.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SVM, RF, MLP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+The wine quality has been forecasted by utilizing ML or AL algorithm of wines that have been generated over 1000 years. Moreover, in an instance, it has been an excellent communication for working out the interaction on among abstract environment of wine &amp; their compound-part. Companies utilize the quality of product certificate for pushing the products &amp; have regard aimed for the unique use of the product. Furthermore, it has been not acceptable for making assured quality by an expert also who is having such high demand aimed at creation due to it might enhance the cost, where the producers of wine pre-requisite ultimate response for streamline average of wine. In this article, correct mines space aimed at simple access &amp; make entire procedure cost-productive &amp; trustworthy utilizing study device. Besides, it enables to model with the system, which estimates the quality of wine by electing significant aspects, which plays a prominent role in defining the quality of the wine. The algorithm of RF has been mined from determining their quality of wine, which might be augmented utilizing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KNN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that uses our projected approach.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,8 +552,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,8 +591,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -542,12 +632,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -575,6 +725,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -860,13 +1034,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,7 +1092,7 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4">
         <v>9</v>
@@ -939,7 +1113,7 @@
     </row>
     <row r="4" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
@@ -960,7 +1134,7 @@
     </row>
     <row r="5" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>8</v>
@@ -1003,7 +1177,7 @@
     </row>
     <row r="7" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
         <v>8</v>
@@ -1023,7 +1197,7 @@
     </row>
     <row r="8" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4">
         <v>8</v>
@@ -1043,7 +1217,7 @@
     </row>
     <row r="9" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
@@ -1063,7 +1237,7 @@
     </row>
     <row r="10" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
@@ -1083,7 +1257,7 @@
     </row>
     <row r="11" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4">
         <v>8</v>
@@ -1103,7 +1277,7 @@
     </row>
     <row r="12" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
         <v>7</v>
@@ -1123,7 +1297,7 @@
     </row>
     <row r="13" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>7</v>
@@ -1143,7 +1317,7 @@
     </row>
     <row r="14" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4">
         <v>7</v>
@@ -1163,7 +1337,7 @@
     </row>
     <row r="15" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>7</v>
@@ -1181,9 +1355,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="231" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>7</v>
@@ -1201,8 +1375,45 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F17" s="5"/>
+    <row r="17" spans="1:6" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="11">
+        <v>7</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" s="15">
+        <v>5</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
@@ -1224,9 +1435,11 @@
     <hyperlink ref="D3" r:id="rId13" xr:uid="{16E08F83-FC71-4447-AB29-37CE62101EE0}"/>
     <hyperlink ref="D11" r:id="rId14" xr:uid="{50F88E45-4A1A-405A-B72C-209E4CC26E44}"/>
     <hyperlink ref="D12" r:id="rId15" xr:uid="{C6C699D6-D80B-47A7-9237-0086697976BF}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{A1962357-0300-4284-9154-CB292915FA3E}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{BC872B7A-ACBF-414D-83DE-44F257C6646B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>